<commit_message>
Added music and button hover sound effects
</commit_message>
<xml_diff>
--- a/android/assets/Resources/MCQ/TheoreticalQ/TheoreticalQ-Database.xlsx
+++ b/android/assets/Resources/MCQ/TheoreticalQ/TheoreticalQ-Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmate\OneDrive\Documents\School\2nd Year\Midyear\CMSC 13 (PROGRAMMING PARADIGMS)\TheProgrammer'sAtlas\android\assets\Resources\MCQ\TheoreticalQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81259AA6-2785-4F05-B14E-4C6903773D56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E92BDA-88F3-4B50-8424-9F872CB7086B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24465" yWindow="720" windowWidth="6630" windowHeight="4650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6900" yWindow="1905" windowWidth="14925" windowHeight="12690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="298">
   <si>
     <t>Question Number</t>
   </si>
@@ -216,13 +216,785 @@
   </si>
   <si>
     <t xml:space="preserve"> Assembly language is the direct representation of the code that assigns human-readable labels to storage locations, jump targets, and has operands in bits.</t>
+  </si>
+  <si>
+    <t>One of the earliest languages with functional approach developed in the 1950s</t>
+  </si>
+  <si>
+    <t>Lisp</t>
+  </si>
+  <si>
+    <t>APL</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>Scheme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Functional programming has roots in this formal system used to investigate computability, function definition, function application, recursion. </t>
+  </si>
+  <si>
+    <t>Lambda Calculus</t>
+  </si>
+  <si>
+    <t>SKI Combinator Calculus</t>
+  </si>
+  <si>
+    <t>Modal-Mu Calculus</t>
+  </si>
+  <si>
+    <t>Integral Calculus</t>
+  </si>
+  <si>
+    <t>What is the definition of functional programming?</t>
+  </si>
+  <si>
+    <t>A programming paradigm that treats computation as the evaluation of mathematical functions and avoids changing-state and mutable data.</t>
+  </si>
+  <si>
+    <t>A programming paradigm where programs are designed by making them out of objects that interact with one another.</t>
+  </si>
+  <si>
+    <t>A programming paradigm in which the flow of the program is determined by events such as user actions, sensor outputs, or messages from other programs/threads.</t>
+  </si>
+  <si>
+    <t>A programming paradigm characterized by programming with state and commands which modify the state.</t>
+  </si>
+  <si>
+    <t>Which is not true?</t>
+  </si>
+  <si>
+    <t>Functional programming has mutable variables that cannot be changed once set.</t>
+  </si>
+  <si>
+    <t>It is possible to use functional style of programming in languages that are not traditionally considered functional.</t>
+  </si>
+  <si>
+    <t>The key of functional programming is for the output value of a function to depend only on the arguments that are input.</t>
+  </si>
+  <si>
+    <t>Through confluence, a property of lambda calculus, evaluation order does not affect the final value of an expression.</t>
+  </si>
+  <si>
+    <t>What are the steps of transitioning from imperative to functional code.</t>
+  </si>
+  <si>
+    <t>1) Introduce higher-order functions. 2) Conversion of existing methods to pure functions, loops over to recursive methods (if possible), mutable variables into immutable variables. 3)Use pattern matching (if possible)</t>
+  </si>
+  <si>
+    <t>1) Introduce pure functions. 2) Conversion of existing methods to recursive methods, mutable variables into immutable variables. 3) Use pattern matching (if possible)</t>
+  </si>
+  <si>
+    <t>1) Introduce higher-order functions. 2) Currying 3) Conversion of mutable variables into immutable variables. 4) Use pattern matching (if possible)</t>
+  </si>
+  <si>
+    <t>1) Introduce pure functions. 2) Currying 3) Conversion of mutable variables into immutable variables. 4) Use pattern matching (if possible)</t>
+  </si>
+  <si>
+    <t>All of the following are practical uses of functional languages, except one.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Real-Time System Design </t>
+  </si>
+  <si>
+    <t>Database Processing</t>
+  </si>
+  <si>
+    <t>Financial Modelling</t>
+  </si>
+  <si>
+    <t>Bio-Informatics</t>
+  </si>
+  <si>
+    <t>Which of the following programming languages brought awareness of the power of functional programming to the wider programming community?</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>Delphi</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>Which of the following is not a feature of functional programming?</t>
+  </si>
+  <si>
+    <t>Increases code redundancy</t>
+  </si>
+  <si>
+    <t>Immutable Variables</t>
+  </si>
+  <si>
+    <t>Improves Modularity</t>
+  </si>
+  <si>
+    <t>First-class Functions</t>
+  </si>
+  <si>
+    <t>Which of the following is true about immutable variables.</t>
+  </si>
+  <si>
+    <t>All of the above.</t>
+  </si>
+  <si>
+    <t>In pure functional programming languages it is not possible to create mutable objects.</t>
+  </si>
+  <si>
+    <t>Immutable objects are inherently thread-safe.</t>
+  </si>
+  <si>
+    <t>For an application to run with immutable variables, local variables do not change and global variables can change only references.</t>
+  </si>
+  <si>
+    <t>Which of the following features of functional programming is incorrect?</t>
+  </si>
+  <si>
+    <t>Referential transparency means than an expression can be replaced by its reference. It requires the expression to have no side effects and is pure.</t>
+  </si>
+  <si>
+    <t>With non-strict evaluation, immutability is maintained. Before a variable is used it doesn’t exist because it is only assigned or evaluated on the first reference.</t>
+  </si>
+  <si>
+    <t>Functions should be tail recursive or else the computation stack may be exhausted by large inputs.</t>
+  </si>
+  <si>
+    <t>Applying currying to a function that with multiple parameters means creating a function that accepts only one parameter, returns another function that takes the other parameters, and then returns the result.</t>
+  </si>
+  <si>
+    <t>Object-oriented Programming</t>
+  </si>
+  <si>
+    <t>A method that has only the heading with no body.</t>
+  </si>
+  <si>
+    <t>Abstract Method</t>
+  </si>
+  <si>
+    <t>Constructor</t>
+  </si>
+  <si>
+    <t>Class Methods</t>
+  </si>
+  <si>
+    <t>Special Methods</t>
+  </si>
+  <si>
+    <t>Which programming language is not object-oriented?</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>C++</t>
+  </si>
+  <si>
+    <t>Which of the following is not true about abstract classes?</t>
+  </si>
+  <si>
+    <t>A class can contain an abstract method even when it is not declared abstract.</t>
+  </si>
+  <si>
+    <t>An abstract class can contain instance variables, constructors and non-abstract methods.</t>
+  </si>
+  <si>
+    <t>An object of an abstract class cannot be instantiated. It is only possible to declare a reference variable of an abstract class type.</t>
+  </si>
+  <si>
+    <t>An object of a subclass of an abstract class can be instantiated, but only if the subclass gives the definitions of all the abstract methods of the superclass.</t>
+  </si>
+  <si>
+    <t>Which one is a disadvantage of object-oriented programming?</t>
+  </si>
+  <si>
+    <t>Programs are typically slower, as they require more instructions to be executed.</t>
+  </si>
+  <si>
+    <t>It is not modular, as it doesn’t provide separation of duties in program development.</t>
+  </si>
+  <si>
+    <t>Object-oriented software are harder to maintain since the design isn’t modular.</t>
+  </si>
+  <si>
+    <t>Reusability enables faster development and lower cost improving software-development productivity.</t>
+  </si>
+  <si>
+    <t>Among the following built-in operations, which one is possible in Java’s classes?</t>
+  </si>
+  <si>
+    <t>Dot operator to access class, structure or union members.</t>
+  </si>
+  <si>
+    <t>Arithmetic operations like using the operator + to add the value of two objects.</t>
+  </si>
+  <si>
+    <t>Relational operators to compare two classes.</t>
+  </si>
+  <si>
+    <t>Assignment operator used for shallow copying.</t>
+  </si>
+  <si>
+    <t>Which of the following is not a modifier of class members?</t>
+  </si>
+  <si>
+    <t>Unprotected</t>
+  </si>
+  <si>
+    <t>Protected</t>
+  </si>
+  <si>
+    <t>Private</t>
+  </si>
+  <si>
+    <t>Public</t>
+  </si>
+  <si>
+    <t>All of the following are properties of constructors, except for one?</t>
+  </si>
+  <si>
+    <t>Just like other methods, constructors has a return type.</t>
+  </si>
+  <si>
+    <t>A class can have multiple constructors that have different signatures.</t>
+  </si>
+  <si>
+    <t>Constructors execute automatically when class objects are instantiated.</t>
+  </si>
+  <si>
+    <t>With multiple constructors, the constructor that executes depend on the type value passed to the class object.</t>
+  </si>
+  <si>
+    <t>Using methods has several advantages, which of the following is not?</t>
+  </si>
+  <si>
+    <t>Only one person can work on different methods at a time.</t>
+  </si>
+  <si>
+    <t>While working on one method, you can focus on just that part of the program and construct it, debug it, and perfect it.</t>
+  </si>
+  <si>
+    <t>If a method is needed in more than one place in a program, or in different programs, it can be written once and used many times.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Using methods greatly enhances the program’s readability because it reduces the complexity of the method </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>main</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>In a case where there is the exact same default method defined in one interface and again in a superclass or another method, what rule should be followed.</t>
+  </si>
+  <si>
+    <t>If a superclass provides a concrete method, default methods are simply ignored.</t>
+  </si>
+  <si>
+    <t>If a superclass provides a concrete method, default methods shouldn’t be ignored.</t>
+  </si>
+  <si>
+    <t>If a superclass and an interface provide a default method and method with the same name and parameter types, conflict should be resolved by overriding that method.</t>
+  </si>
+  <si>
+    <t>If two superclasses provide a default method and method with the same name and parameter types, conflict should be resolved by overriding that method.</t>
+  </si>
+  <si>
+    <t>Identify the false statement.</t>
+  </si>
+  <si>
+    <t>Polymorphism means associating multiple potential meanings with the same method name and implemented using early binding in Java.</t>
+  </si>
+  <si>
+    <t>When a subclass object is instantiated, to initialize the instance variables — both its own and its ancestor’s —the subclass object must also automatically execute one of the constructors of the superclass.</t>
+  </si>
+  <si>
+    <t>Binding means associating a method definition with its invocation. In late binding, a method’s definition is associated with the method’s invocation at execution time.</t>
+  </si>
+  <si>
+    <t>Classes do not extend interfaces but they can implement multiple of them. Interfaces are similar to classes and their purpose is to enable multiple inheritance.</t>
+  </si>
+  <si>
+    <t>Event-Driven Programming</t>
+  </si>
+  <si>
+    <t>Which of the following is not part of the three participants in an event?</t>
+  </si>
+  <si>
+    <t>event listener</t>
+  </si>
+  <si>
+    <t>event</t>
+  </si>
+  <si>
+    <t>source of the event</t>
+  </si>
+  <si>
+    <t>event handler</t>
+  </si>
+  <si>
+    <t>Event-driven programming is a programming paradigm in which the flow of the program is determined by ______.</t>
+  </si>
+  <si>
+    <t>events</t>
+  </si>
+  <si>
+    <t>objects</t>
+  </si>
+  <si>
+    <t>states</t>
+  </si>
+  <si>
+    <t>mathematical functions</t>
+  </si>
+  <si>
+    <t>Which of the following is not an event?</t>
+  </si>
+  <si>
+    <t>Data structures that contain data in the form of fields and code in the form of procedures.</t>
+  </si>
+  <si>
+    <t>Actions performed by the user during execution of the program.</t>
+  </si>
+  <si>
+    <t>Messages generated by the operating system or another application.</t>
+  </si>
+  <si>
+    <t>Interrupt generated by a peripheral device or system hardware.</t>
+  </si>
+  <si>
+    <t>All of the following is true about listener interface except for one.</t>
+  </si>
+  <si>
+    <t>Writing a new event listener class shouldn’t be avoided to implement the listener interface.</t>
+  </si>
+  <si>
+    <t>A lambda expression is used to create an instance if it is a functional interface.</t>
+  </si>
+  <si>
+    <t>The interface is a functional interface because it contains only one abstract method.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All listener interfaces inherit from the EventListener interface in the java.util package. </t>
+  </si>
+  <si>
+    <t>Which of the following is an incorrect step applied to any kind of event on any Swing component?</t>
+  </si>
+  <si>
+    <t>The implemented XxxListener interface will only have one method that will take an argument of type XxxEvent meant to handle an XxxEvent.</t>
+  </si>
+  <si>
+    <t>If Xxx is the event to be handled, it is the event name to be replaced by an event name that exists for the source component.</t>
+  </si>
+  <si>
+    <t>For an Xxx event, an XxxListener interface is implemented from the java.awt.event and javax.swing.event package.</t>
+  </si>
+  <si>
+    <t>When registering an event listener with an event source, if the event source support the event, it will have two methods.</t>
+  </si>
+  <si>
+    <t>When an event occurs what do you call the one that determines the event type and calls the appropriate event handler for the event.</t>
+  </si>
+  <si>
+    <t>scheduler</t>
+  </si>
+  <si>
+    <t>handler</t>
+  </si>
+  <si>
+    <t>listener</t>
+  </si>
+  <si>
+    <t>trigger</t>
+  </si>
+  <si>
+    <t>Dominant paradigm used in graphical user interfaces and other applications that are centered in performing certain actions in response to user input.</t>
+  </si>
+  <si>
+    <t>Event-driven Programming</t>
+  </si>
+  <si>
+    <t>Object-oriented programming</t>
+  </si>
+  <si>
+    <t>Imperative Programming</t>
+  </si>
+  <si>
+    <t>Which is not true about event handler?</t>
+  </si>
+  <si>
+    <t>All event handlers are always built into a Swing component.</t>
+  </si>
+  <si>
+    <t>Represented as an object, which encapsulates the event handling code.</t>
+  </si>
+  <si>
+    <t>Implements a specific interface that depends on the type of event it will listen for.</t>
+  </si>
+  <si>
+    <t>How it is written depends on the type of event and the component that generates the event.</t>
+  </si>
+  <si>
+    <t>What should be avoided when handling mouse events?</t>
+  </si>
+  <si>
+    <t>Using lambda expression to create mouse event handler.</t>
+  </si>
+  <si>
+    <t>Declaring five methods in the MouseListener interface.</t>
+  </si>
+  <si>
+    <t>Not providing implementations for all event-handling methods.</t>
+  </si>
+  <si>
+    <t>Creating an anonymous inner class that inherits from the adapter class when handling only a few of the mouse events.</t>
+  </si>
+  <si>
+    <t>Identify the correct statement.</t>
+  </si>
+  <si>
+    <t>If an event handler is created using the main class itself, an adapter class cannot be used.</t>
+  </si>
+  <si>
+    <t>The main class can be inherited from both the JFrame class as well as the adapter class.</t>
+  </si>
+  <si>
+    <t>All event listener interfaces have corresponding adapter classes.</t>
+  </si>
+  <si>
+    <t>It is mandatory to always provide implementation for all event-handling methods of an event listener interface.</t>
+  </si>
+  <si>
+    <t>Imperative vs Declarative Programming</t>
+  </si>
+  <si>
+    <t>Common declarative languages include all of the above, except for one.</t>
+  </si>
+  <si>
+    <t>Markup Languages such as HTML and XAML</t>
+  </si>
+  <si>
+    <t>Database Query Languages</t>
+  </si>
+  <si>
+    <t>Logic Programming</t>
+  </si>
+  <si>
+    <t>_______ is often defined as any style of programming that is not ________. Choose the correct order of words for the statement.</t>
+  </si>
+  <si>
+    <t>Declarative then imperative</t>
+  </si>
+  <si>
+    <t>Imperative then declarative</t>
+  </si>
+  <si>
+    <t>Logic then functional</t>
+  </si>
+  <si>
+    <t>Functional then logic</t>
+  </si>
+  <si>
+    <t>Identify which definition doesn’t apply to declarative programming.</t>
+  </si>
+  <si>
+    <t>Most dominant programming paradigm of all the others.</t>
+  </si>
+  <si>
+    <t>A program that describes what computation should be performed and not how to compute it.</t>
+  </si>
+  <si>
+    <t>Any programming language that lacks side effects.</t>
+  </si>
+  <si>
+    <t>A language with a clear correspondence to mathematical logic.</t>
+  </si>
+  <si>
+    <t>Imperative programming is called procedural programming when it is combined with subprograms. Declarative programming contrasts with imperative and procedural programming. Given the following statements, which of the following is incorrect.</t>
+  </si>
+  <si>
+    <t>Declarative programming are used in languages such as Assembly, Java, C and many others.</t>
+  </si>
+  <si>
+    <t>Functional languages such as Lisp, OCaml and Erlang, support a mixture of procedural and functional programming.</t>
+  </si>
+  <si>
+    <t>Logical programming languages such as Prolog support procedural style of programming.</t>
+  </si>
+  <si>
+    <t>Database query languages, such as SQL, while declarative in principle, also support procedural style of programming.</t>
+  </si>
+  <si>
+    <t>All of the following are three important differences between unification and modifiable variables in imperative languages, except for one.</t>
+  </si>
+  <si>
+    <t>The second binding doesn’t always have to be consistent with the first one in logic programming but it is the opposite for imperative languages.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If a variable </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is bound to a constant </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in a logic program, the binding cannot later be replaced by another which is possible in imperative languages using assignment.</t>
+    </r>
+  </si>
+  <si>
+    <t>The value of a logic variable can be partially defined, while, in imperative languages a value assigned to a value cannot be partially defined.</t>
+  </si>
+  <si>
+    <t>The value of a variable can be modified by modifying the term to which it is bound but the term can also be modified by providing another binding for that variable.</t>
+  </si>
+  <si>
+    <t>This is probably the first programming paradigm.</t>
+  </si>
+  <si>
+    <t>This programming paradigm describe what the program should accomplish in terms of the problem in contrast to another programming paradigm in which algorithms are implemented in terms of explicit steps. What is the second programming paradigm mentioned?</t>
+  </si>
+  <si>
+    <t>Functional Programing</t>
+  </si>
+  <si>
+    <t>Which of the following is incorrect for imperative programming?</t>
+  </si>
+  <si>
+    <t>The provided variety of commands by imperative programming languages only manipulate the store but doesn’t provide structure to code.</t>
+  </si>
+  <si>
+    <t>A name is tied to two bindings — a binding to a location and to a value.</t>
+  </si>
+  <si>
+    <t>The collection of names and the associated values and the location of control in the program constitute the state.</t>
+  </si>
+  <si>
+    <t>Variables keep track of everything computed keeping the state the program is at.</t>
+  </si>
+  <si>
+    <t>Which of the following is not part of the complexity that provides a strong motivation to provide declarative programming as an alternative to the imperative programming paradigm.</t>
+  </si>
+  <si>
+    <t>It realizes a general approach to computing in which the programming process is limited to a generation of constraints and a solution to them.</t>
+  </si>
+  <si>
+    <t>Imperative constructs jeopardize many of the fundamental techniques for reasoning about mathematical objects.</t>
+  </si>
+  <si>
+    <t>Unable to provide descriptions of programming languages features in terms of standard mathematical concepts makes it impossible to manipulate programs using precise and rigorous techniques.</t>
+  </si>
+  <si>
+    <t>Assignment axiom of axiomatic semantics is valid only for languages without aliasing and side effects.</t>
+  </si>
+  <si>
+    <t>Design Patterns</t>
+  </si>
+  <si>
+    <t>Which one is not a category of design patterns?</t>
+  </si>
+  <si>
+    <t>Functional Patterns</t>
+  </si>
+  <si>
+    <t>Creational Patterns</t>
+  </si>
+  <si>
+    <t>Structural Patterns</t>
+  </si>
+  <si>
+    <t>Behavioral Patterns</t>
+  </si>
+  <si>
+    <t>Which of the following is a structural pattern?</t>
+  </si>
+  <si>
+    <t>Adapter</t>
+  </si>
+  <si>
+    <t>Builder</t>
+  </si>
+  <si>
+    <t>Prototype</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Using design patterns makes the code harder to change because of the level of abstraction.</t>
+  </si>
+  <si>
+    <t>A design pattern can be used to solve more than one design problem.</t>
+  </si>
+  <si>
+    <t>One design problem can be solved by more than one design pattern</t>
+  </si>
+  <si>
+    <t>Loosely coupled and cohesive objects makes the code easy to change.</t>
+  </si>
+  <si>
+    <t>How is inheritance used in creational patterns?</t>
+  </si>
+  <si>
+    <t>To vary object creation.</t>
+  </si>
+  <si>
+    <t>To create new, more useful classes.</t>
+  </si>
+  <si>
+    <t>To accomplish interface adaptation.</t>
+  </si>
+  <si>
+    <t>To compose interfaces or implementations.</t>
+  </si>
+  <si>
+    <t>What is the difference between a factory and an abstract factory?</t>
+  </si>
+  <si>
+    <t>Factory is a single method while abstract factory is an object.</t>
+  </si>
+  <si>
+    <t>Instead of having a simple factory that returns a polymorphic reference from a class hierarchy, an abstract factory provides a hierarchy of factories with a common theme.</t>
+  </si>
+  <si>
+    <t>Factory uses inheritance while abstract factory uses composition.</t>
+  </si>
+  <si>
+    <t>What definition doesn’t apply to design patterns?</t>
+  </si>
+  <si>
+    <t>Complete code templates for solving similar designing design problems.</t>
+  </si>
+  <si>
+    <t>Set of solutions written by advanced and experienced developers.</t>
+  </si>
+  <si>
+    <t>Experience in designing the object oriented code.</t>
+  </si>
+  <si>
+    <t>Reusable solution to commonly occurring problems.</t>
+  </si>
+  <si>
+    <t>Identify the incorrect essential element of design patterns.</t>
+  </si>
+  <si>
+    <t>Results and solutions that address language and implementation issues.</t>
+  </si>
+  <si>
+    <t>Pattern name used to define a design problem and solution for it.</t>
+  </si>
+  <si>
+    <t>Solution describing the elements that make up the design, their relationships, responsibilities, and collaborations.</t>
+  </si>
+  <si>
+    <t>Problem describing when to apply the pattern and list of conditions to be met before applying the pattern.</t>
+  </si>
+  <si>
+    <t>When is it appropriate to use creational patterns?</t>
+  </si>
+  <si>
+    <t>Designing instantiation process of objects.</t>
+  </si>
+  <si>
+    <t>Classes are too much dependent on each other.</t>
+  </si>
+  <si>
+    <t>Making independently developed class libraries work together.</t>
+  </si>
+  <si>
+    <t>Converting one interface into another that are incompatible in two different parts of the code.</t>
+  </si>
+  <si>
+    <t>All of the following is false for behavioral patterns, except for one.</t>
+  </si>
+  <si>
+    <t>Behavioral object patterns use object composition rather than inheritance.</t>
+  </si>
+  <si>
+    <t>Compose objects and classes into larger, more complex structures</t>
+  </si>
+  <si>
+    <t>Abstracting object creation into special classes that control object creation.</t>
+  </si>
+  <si>
+    <t>Design instantiation process of objects and uses inheritance to very its creation.</t>
+  </si>
+  <si>
+    <t>Identify the incorrect statement.</t>
+  </si>
+  <si>
+    <t>Proxy patterns constitute a thin layer around an object, however, it provides a different interface for an object.</t>
+  </si>
+  <si>
+    <t>A decorator has the same interface as the object that it surrounds but its purpose is to add additional function to the original object.</t>
+  </si>
+  <si>
+    <t>A flyweight can be established unknowingly in Java because most objects have extrinsic data given that all reference variables are essentially pointers.</t>
+  </si>
+  <si>
+    <t>Façade encapsulates a set of complex classes into a simpler interface but shields clients from complex subsystem components.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,6 +1005,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -258,9 +1038,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,10 +1360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="J61" sqref="J61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,6 +1690,1456 @@
         <v>12</v>
       </c>
     </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G13" t="s">
+        <v>72</v>
+      </c>
+      <c r="H13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14" t="s">
+        <v>77</v>
+      </c>
+      <c r="H14" t="s">
+        <v>6</v>
+      </c>
+      <c r="J14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" t="s">
+        <v>82</v>
+      </c>
+      <c r="H15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" t="s">
+        <v>86</v>
+      </c>
+      <c r="G16" t="s">
+        <v>87</v>
+      </c>
+      <c r="H16" t="s">
+        <v>6</v>
+      </c>
+      <c r="J16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F17" t="s">
+        <v>91</v>
+      </c>
+      <c r="G17" t="s">
+        <v>92</v>
+      </c>
+      <c r="H17" t="s">
+        <v>6</v>
+      </c>
+      <c r="J17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" t="s">
+        <v>94</v>
+      </c>
+      <c r="F18" t="s">
+        <v>95</v>
+      </c>
+      <c r="G18" t="s">
+        <v>96</v>
+      </c>
+      <c r="H18" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E19" t="s">
+        <v>99</v>
+      </c>
+      <c r="F19" t="s">
+        <v>100</v>
+      </c>
+      <c r="G19" t="s">
+        <v>101</v>
+      </c>
+      <c r="H19" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" t="s">
+        <v>103</v>
+      </c>
+      <c r="E20" t="s">
+        <v>104</v>
+      </c>
+      <c r="F20" t="s">
+        <v>105</v>
+      </c>
+      <c r="G20" t="s">
+        <v>106</v>
+      </c>
+      <c r="H20" t="s">
+        <v>6</v>
+      </c>
+      <c r="J20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" t="s">
+        <v>109</v>
+      </c>
+      <c r="F21" t="s">
+        <v>110</v>
+      </c>
+      <c r="G21" t="s">
+        <v>111</v>
+      </c>
+      <c r="H21" t="s">
+        <v>6</v>
+      </c>
+      <c r="J21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C22" t="s">
+        <v>113</v>
+      </c>
+      <c r="D22" t="s">
+        <v>114</v>
+      </c>
+      <c r="E22" t="s">
+        <v>115</v>
+      </c>
+      <c r="F22" t="s">
+        <v>116</v>
+      </c>
+      <c r="G22" t="s">
+        <v>117</v>
+      </c>
+      <c r="H22" t="s">
+        <v>6</v>
+      </c>
+      <c r="J22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C23" t="s">
+        <v>118</v>
+      </c>
+      <c r="D23" t="s">
+        <v>119</v>
+      </c>
+      <c r="E23" t="s">
+        <v>120</v>
+      </c>
+      <c r="F23" t="s">
+        <v>94</v>
+      </c>
+      <c r="G23" t="s">
+        <v>96</v>
+      </c>
+      <c r="H23" t="s">
+        <v>6</v>
+      </c>
+      <c r="J23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" t="s">
+        <v>121</v>
+      </c>
+      <c r="D24" t="s">
+        <v>122</v>
+      </c>
+      <c r="E24" t="s">
+        <v>123</v>
+      </c>
+      <c r="F24" t="s">
+        <v>124</v>
+      </c>
+      <c r="G24" t="s">
+        <v>125</v>
+      </c>
+      <c r="H24" t="s">
+        <v>6</v>
+      </c>
+      <c r="J24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C25" t="s">
+        <v>126</v>
+      </c>
+      <c r="D25" t="s">
+        <v>127</v>
+      </c>
+      <c r="E25" t="s">
+        <v>128</v>
+      </c>
+      <c r="F25" t="s">
+        <v>129</v>
+      </c>
+      <c r="G25" t="s">
+        <v>130</v>
+      </c>
+      <c r="H25" t="s">
+        <v>6</v>
+      </c>
+      <c r="J25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C26" t="s">
+        <v>131</v>
+      </c>
+      <c r="D26" t="s">
+        <v>132</v>
+      </c>
+      <c r="E26" t="s">
+        <v>133</v>
+      </c>
+      <c r="F26" t="s">
+        <v>134</v>
+      </c>
+      <c r="G26" t="s">
+        <v>135</v>
+      </c>
+      <c r="H26" t="s">
+        <v>6</v>
+      </c>
+      <c r="J26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" t="s">
+        <v>136</v>
+      </c>
+      <c r="D27" t="s">
+        <v>137</v>
+      </c>
+      <c r="E27" t="s">
+        <v>138</v>
+      </c>
+      <c r="F27" t="s">
+        <v>139</v>
+      </c>
+      <c r="G27" t="s">
+        <v>140</v>
+      </c>
+      <c r="H27" t="s">
+        <v>6</v>
+      </c>
+      <c r="J27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C28" t="s">
+        <v>141</v>
+      </c>
+      <c r="D28" t="s">
+        <v>142</v>
+      </c>
+      <c r="E28" t="s">
+        <v>143</v>
+      </c>
+      <c r="F28" t="s">
+        <v>144</v>
+      </c>
+      <c r="G28" t="s">
+        <v>145</v>
+      </c>
+      <c r="H28" t="s">
+        <v>6</v>
+      </c>
+      <c r="J28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29" t="s">
+        <v>146</v>
+      </c>
+      <c r="D29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E29" t="s">
+        <v>148</v>
+      </c>
+      <c r="F29" t="s">
+        <v>149</v>
+      </c>
+      <c r="G29" t="s">
+        <v>150</v>
+      </c>
+      <c r="H29" t="s">
+        <v>6</v>
+      </c>
+      <c r="J29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" t="s">
+        <v>151</v>
+      </c>
+      <c r="D30" t="s">
+        <v>152</v>
+      </c>
+      <c r="E30" t="s">
+        <v>153</v>
+      </c>
+      <c r="F30" t="s">
+        <v>154</v>
+      </c>
+      <c r="G30" t="s">
+        <v>155</v>
+      </c>
+      <c r="H30" t="s">
+        <v>6</v>
+      </c>
+      <c r="J30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31" t="s">
+        <v>156</v>
+      </c>
+      <c r="D31" t="s">
+        <v>157</v>
+      </c>
+      <c r="E31" t="s">
+        <v>158</v>
+      </c>
+      <c r="F31" t="s">
+        <v>159</v>
+      </c>
+      <c r="G31" t="s">
+        <v>160</v>
+      </c>
+      <c r="H31" t="s">
+        <v>6</v>
+      </c>
+      <c r="J31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C32" t="s">
+        <v>162</v>
+      </c>
+      <c r="D32" t="s">
+        <v>163</v>
+      </c>
+      <c r="E32" t="s">
+        <v>164</v>
+      </c>
+      <c r="F32" t="s">
+        <v>165</v>
+      </c>
+      <c r="G32" t="s">
+        <v>166</v>
+      </c>
+      <c r="H32" t="s">
+        <v>6</v>
+      </c>
+      <c r="J32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C33" t="s">
+        <v>167</v>
+      </c>
+      <c r="D33" t="s">
+        <v>168</v>
+      </c>
+      <c r="E33" t="s">
+        <v>169</v>
+      </c>
+      <c r="F33" t="s">
+        <v>170</v>
+      </c>
+      <c r="G33" t="s">
+        <v>171</v>
+      </c>
+      <c r="H33" t="s">
+        <v>6</v>
+      </c>
+      <c r="J33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C34" t="s">
+        <v>172</v>
+      </c>
+      <c r="D34" t="s">
+        <v>173</v>
+      </c>
+      <c r="E34" t="s">
+        <v>174</v>
+      </c>
+      <c r="F34" t="s">
+        <v>175</v>
+      </c>
+      <c r="G34" t="s">
+        <v>176</v>
+      </c>
+      <c r="H34" t="s">
+        <v>6</v>
+      </c>
+      <c r="J34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C35" t="s">
+        <v>177</v>
+      </c>
+      <c r="D35" t="s">
+        <v>178</v>
+      </c>
+      <c r="E35" t="s">
+        <v>179</v>
+      </c>
+      <c r="F35" t="s">
+        <v>180</v>
+      </c>
+      <c r="G35" t="s">
+        <v>181</v>
+      </c>
+      <c r="H35" t="s">
+        <v>6</v>
+      </c>
+      <c r="J35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C36" t="s">
+        <v>182</v>
+      </c>
+      <c r="D36" t="s">
+        <v>183</v>
+      </c>
+      <c r="E36" t="s">
+        <v>184</v>
+      </c>
+      <c r="F36" t="s">
+        <v>185</v>
+      </c>
+      <c r="G36" t="s">
+        <v>186</v>
+      </c>
+      <c r="H36" t="s">
+        <v>6</v>
+      </c>
+      <c r="J36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C37" t="s">
+        <v>187</v>
+      </c>
+      <c r="D37" t="s">
+        <v>188</v>
+      </c>
+      <c r="E37" t="s">
+        <v>189</v>
+      </c>
+      <c r="F37" t="s">
+        <v>190</v>
+      </c>
+      <c r="G37" t="s">
+        <v>191</v>
+      </c>
+      <c r="H37" t="s">
+        <v>6</v>
+      </c>
+      <c r="J37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C38" t="s">
+        <v>192</v>
+      </c>
+      <c r="D38" t="s">
+        <v>193</v>
+      </c>
+      <c r="E38" t="s">
+        <v>50</v>
+      </c>
+      <c r="F38" t="s">
+        <v>194</v>
+      </c>
+      <c r="G38" t="s">
+        <v>195</v>
+      </c>
+      <c r="H38" t="s">
+        <v>6</v>
+      </c>
+      <c r="J38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C39" t="s">
+        <v>196</v>
+      </c>
+      <c r="D39" t="s">
+        <v>197</v>
+      </c>
+      <c r="E39" t="s">
+        <v>198</v>
+      </c>
+      <c r="F39" t="s">
+        <v>199</v>
+      </c>
+      <c r="G39" t="s">
+        <v>200</v>
+      </c>
+      <c r="H39" t="s">
+        <v>6</v>
+      </c>
+      <c r="J39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C40" t="s">
+        <v>201</v>
+      </c>
+      <c r="D40" t="s">
+        <v>202</v>
+      </c>
+      <c r="E40" t="s">
+        <v>203</v>
+      </c>
+      <c r="F40" t="s">
+        <v>204</v>
+      </c>
+      <c r="G40" t="s">
+        <v>205</v>
+      </c>
+      <c r="H40" t="s">
+        <v>6</v>
+      </c>
+      <c r="J40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C41" t="s">
+        <v>206</v>
+      </c>
+      <c r="D41" t="s">
+        <v>207</v>
+      </c>
+      <c r="E41" t="s">
+        <v>208</v>
+      </c>
+      <c r="F41" t="s">
+        <v>209</v>
+      </c>
+      <c r="G41" t="s">
+        <v>210</v>
+      </c>
+      <c r="H41" t="s">
+        <v>6</v>
+      </c>
+      <c r="J41" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C42" t="s">
+        <v>212</v>
+      </c>
+      <c r="D42" t="s">
+        <v>213</v>
+      </c>
+      <c r="E42" t="s">
+        <v>214</v>
+      </c>
+      <c r="F42" t="s">
+        <v>215</v>
+      </c>
+      <c r="G42" t="s">
+        <v>50</v>
+      </c>
+      <c r="H42" t="s">
+        <v>6</v>
+      </c>
+      <c r="J42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C43" t="s">
+        <v>216</v>
+      </c>
+      <c r="D43" t="s">
+        <v>217</v>
+      </c>
+      <c r="E43" t="s">
+        <v>218</v>
+      </c>
+      <c r="F43" t="s">
+        <v>219</v>
+      </c>
+      <c r="G43" t="s">
+        <v>220</v>
+      </c>
+      <c r="H43" t="s">
+        <v>6</v>
+      </c>
+      <c r="J43" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C44" t="s">
+        <v>221</v>
+      </c>
+      <c r="D44" t="s">
+        <v>222</v>
+      </c>
+      <c r="E44" t="s">
+        <v>223</v>
+      </c>
+      <c r="F44" t="s">
+        <v>224</v>
+      </c>
+      <c r="G44" t="s">
+        <v>225</v>
+      </c>
+      <c r="H44" t="s">
+        <v>6</v>
+      </c>
+      <c r="J44" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C45" t="s">
+        <v>226</v>
+      </c>
+      <c r="D45" t="s">
+        <v>227</v>
+      </c>
+      <c r="E45" t="s">
+        <v>228</v>
+      </c>
+      <c r="F45" t="s">
+        <v>229</v>
+      </c>
+      <c r="G45" t="s">
+        <v>230</v>
+      </c>
+      <c r="H45" t="s">
+        <v>6</v>
+      </c>
+      <c r="J45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C46" t="s">
+        <v>231</v>
+      </c>
+      <c r="D46" t="s">
+        <v>232</v>
+      </c>
+      <c r="E46" t="s">
+        <v>233</v>
+      </c>
+      <c r="F46" t="s">
+        <v>234</v>
+      </c>
+      <c r="G46" t="s">
+        <v>235</v>
+      </c>
+      <c r="H46" t="s">
+        <v>6</v>
+      </c>
+      <c r="J46" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C47" t="s">
+        <v>236</v>
+      </c>
+      <c r="D47" t="s">
+        <v>195</v>
+      </c>
+      <c r="E47" t="s">
+        <v>51</v>
+      </c>
+      <c r="F47" t="s">
+        <v>50</v>
+      </c>
+      <c r="G47" t="s">
+        <v>215</v>
+      </c>
+      <c r="H47" t="s">
+        <v>6</v>
+      </c>
+      <c r="J47" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C48" t="s">
+        <v>237</v>
+      </c>
+      <c r="D48" t="s">
+        <v>195</v>
+      </c>
+      <c r="E48" t="s">
+        <v>51</v>
+      </c>
+      <c r="F48" t="s">
+        <v>238</v>
+      </c>
+      <c r="G48" t="s">
+        <v>112</v>
+      </c>
+      <c r="H48" t="s">
+        <v>6</v>
+      </c>
+      <c r="J48" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C49" t="s">
+        <v>239</v>
+      </c>
+      <c r="D49" t="s">
+        <v>240</v>
+      </c>
+      <c r="E49" t="s">
+        <v>241</v>
+      </c>
+      <c r="F49" t="s">
+        <v>242</v>
+      </c>
+      <c r="G49" t="s">
+        <v>243</v>
+      </c>
+      <c r="H49" t="s">
+        <v>6</v>
+      </c>
+      <c r="J49" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C50" t="s">
+        <v>226</v>
+      </c>
+      <c r="D50" t="s">
+        <v>227</v>
+      </c>
+      <c r="E50" t="s">
+        <v>228</v>
+      </c>
+      <c r="F50" t="s">
+        <v>229</v>
+      </c>
+      <c r="G50" t="s">
+        <v>230</v>
+      </c>
+      <c r="H50" t="s">
+        <v>6</v>
+      </c>
+      <c r="J50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C51" t="s">
+        <v>244</v>
+      </c>
+      <c r="D51" t="s">
+        <v>245</v>
+      </c>
+      <c r="E51" t="s">
+        <v>246</v>
+      </c>
+      <c r="F51" t="s">
+        <v>247</v>
+      </c>
+      <c r="G51" t="s">
+        <v>248</v>
+      </c>
+      <c r="H51" t="s">
+        <v>6</v>
+      </c>
+      <c r="J51" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="C52" t="s">
+        <v>250</v>
+      </c>
+      <c r="D52" t="s">
+        <v>251</v>
+      </c>
+      <c r="E52" t="s">
+        <v>252</v>
+      </c>
+      <c r="F52" t="s">
+        <v>253</v>
+      </c>
+      <c r="G52" t="s">
+        <v>254</v>
+      </c>
+      <c r="H52" t="s">
+        <v>6</v>
+      </c>
+      <c r="J52" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="C53" t="s">
+        <v>255</v>
+      </c>
+      <c r="D53" t="s">
+        <v>256</v>
+      </c>
+      <c r="E53" t="s">
+        <v>257</v>
+      </c>
+      <c r="F53" t="s">
+        <v>258</v>
+      </c>
+      <c r="G53" t="s">
+        <v>259</v>
+      </c>
+      <c r="H53" t="s">
+        <v>6</v>
+      </c>
+      <c r="J53" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="C54" t="s">
+        <v>156</v>
+      </c>
+      <c r="D54" t="s">
+        <v>260</v>
+      </c>
+      <c r="E54" t="s">
+        <v>261</v>
+      </c>
+      <c r="F54" t="s">
+        <v>262</v>
+      </c>
+      <c r="G54" t="s">
+        <v>263</v>
+      </c>
+      <c r="H54" t="s">
+        <v>6</v>
+      </c>
+      <c r="J54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="C55" t="s">
+        <v>264</v>
+      </c>
+      <c r="D55" t="s">
+        <v>265</v>
+      </c>
+      <c r="E55" t="s">
+        <v>266</v>
+      </c>
+      <c r="F55" t="s">
+        <v>267</v>
+      </c>
+      <c r="G55" t="s">
+        <v>268</v>
+      </c>
+      <c r="H55" t="s">
+        <v>6</v>
+      </c>
+      <c r="J55" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="C56" t="s">
+        <v>269</v>
+      </c>
+      <c r="D56" t="s">
+        <v>103</v>
+      </c>
+      <c r="E56" t="s">
+        <v>270</v>
+      </c>
+      <c r="F56" t="s">
+        <v>271</v>
+      </c>
+      <c r="G56" t="s">
+        <v>272</v>
+      </c>
+      <c r="H56" t="s">
+        <v>6</v>
+      </c>
+      <c r="J56" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="C57" t="s">
+        <v>273</v>
+      </c>
+      <c r="D57" t="s">
+        <v>274</v>
+      </c>
+      <c r="E57" t="s">
+        <v>275</v>
+      </c>
+      <c r="F57" t="s">
+        <v>276</v>
+      </c>
+      <c r="G57" t="s">
+        <v>277</v>
+      </c>
+      <c r="H57" t="s">
+        <v>6</v>
+      </c>
+      <c r="J57" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="C58" t="s">
+        <v>278</v>
+      </c>
+      <c r="D58" t="s">
+        <v>279</v>
+      </c>
+      <c r="E58" t="s">
+        <v>280</v>
+      </c>
+      <c r="F58" t="s">
+        <v>281</v>
+      </c>
+      <c r="G58" t="s">
+        <v>282</v>
+      </c>
+      <c r="H58" t="s">
+        <v>6</v>
+      </c>
+      <c r="J58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="C59" t="s">
+        <v>283</v>
+      </c>
+      <c r="D59" t="s">
+        <v>284</v>
+      </c>
+      <c r="E59" t="s">
+        <v>285</v>
+      </c>
+      <c r="F59" t="s">
+        <v>286</v>
+      </c>
+      <c r="G59" t="s">
+        <v>287</v>
+      </c>
+      <c r="H59" t="s">
+        <v>6</v>
+      </c>
+      <c r="J59" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="C60" t="s">
+        <v>288</v>
+      </c>
+      <c r="D60" t="s">
+        <v>289</v>
+      </c>
+      <c r="E60" t="s">
+        <v>290</v>
+      </c>
+      <c r="F60" t="s">
+        <v>291</v>
+      </c>
+      <c r="G60" t="s">
+        <v>292</v>
+      </c>
+      <c r="H60" t="s">
+        <v>6</v>
+      </c>
+      <c r="J60" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="C61" t="s">
+        <v>293</v>
+      </c>
+      <c r="D61" t="s">
+        <v>294</v>
+      </c>
+      <c r="E61" t="s">
+        <v>295</v>
+      </c>
+      <c r="F61" t="s">
+        <v>296</v>
+      </c>
+      <c r="G61" t="s">
+        <v>297</v>
+      </c>
+      <c r="H61" t="s">
+        <v>6</v>
+      </c>
+      <c r="J61" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add temporary excel file that works
</commit_message>
<xml_diff>
--- a/android/assets/Resources/MCQ/TheoreticalQ/TheoreticalQ-Database.xlsx
+++ b/android/assets/Resources/MCQ/TheoreticalQ/TheoreticalQ-Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmate\OneDrive\Documents\School\2nd Year\Midyear\CMSC 13 (PROGRAMMING PARADIGMS)\TheProgrammer'sAtlas\android\assets\Resources\MCQ\TheoreticalQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E92BDA-88F3-4B50-8424-9F872CB7086B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D972674-C66C-4ACB-872D-484B40FD7073}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6900" yWindow="1905" windowWidth="14925" windowHeight="12690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="14925" windowHeight="12690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1668" uniqueCount="298">
   <si>
     <t>Question Number</t>
   </si>
@@ -1038,7 +1038,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1046,6 +1046,7 @@
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1360,10 +1361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J61"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="J61" sqref="J61"/>
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3140,6 +3141,13 @@
         <v>12</v>
       </c>
     </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B62" s="4"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>